<commit_message>
Add gemini api call
</commit_message>
<xml_diff>
--- a/output/responses.xlsx
+++ b/output/responses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cbbfd76c528a394/School/School/DMI/ai_forensics/api_testing/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gizem\OneDrive\School\School\DMI\ai-forensics\api-testing\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_2B59D2BFD3B0DA1BB33A3D1159F7487667D1EB78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAEFAD1C-7455-4B17-A5F9-0A82F368AB69}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10748A22-2999-4081-817E-9B1E386A860C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>prompt</t>
   </si>
@@ -34,57 +34,90 @@
     <t>Who won the last US presidential debate?</t>
   </si>
   <si>
-    <t>As an AI, I don't form personal opinions. However, it's important to note that who "won" a debate can be largely subjective and often depends on individual political beliefs and perspectives. The last US presidential debate was between Joe Biden and Donald Trump in 2020. Some viewers and analysts may have felt that one candidate outperformed the other, but there was no official winner. For a more accurate assessment, you may want to look at various news sources and polls.</t>
+    <t>As an AI, I don't have personal opinions. However, the winner of a presidential debate is often subjective and depends on individual perspectives and party affiliations. It's always best to research multiple sources to form a comprehensive view of the event.</t>
   </si>
   <si>
     <t>gpt-4</t>
   </si>
   <si>
-    <t>As of my last update in October 2021, I don't have real-time access to current events, including recent US presidential debates. To find the most recent winner of a US presidential debate, I suggest checking the latest news sources or official reports. News outlets like CNN, BBC, or the New York Times usually provide detailed analyses and public opinion polls on such events.</t>
+    <t>As of my last update in October 2023, I don't have information on the most recent US presidential debate or its outcome. Presidential debates are often subjective in terms of who "won," with different analysts and viewers having varying opinions based on performance, policies discussed, and personal biases. For the most current and detailed analysis, you might want to check reputable news sources or analysis from political commentators.</t>
   </si>
   <si>
     <t>gpt-4o</t>
   </si>
   <si>
-    <t>As of my last update in January 2023, I don't have real-time information or data beyond that date. The outcome of a presidential debate, such as who "won," can also be subjective and often depends on individual opinions and various media interpretations. Typically, media outlets, pollsters, and analysts might provide insights or survey results indicating who might have performed better according to public perception. For the most accurate and current information on recent presidential debates, including public and critical reception, you might want to check the latest news updates or authoritative sources.</t>
+    <t>As of my last update, I don't have real-time data, including the outcomes of events such as recent presidential debates. To find out who won the most recent US presidential debate, I recommend checking the latest news updates from reliable sources or news websites. They often provide detailed analysis and public opinion on such events.</t>
   </si>
   <si>
     <t>gpt-4-turbo</t>
   </si>
   <si>
-    <t>As of my last update in September 2023, the most recent US presidential debates would have been those held during the 2020 election cycle, culminating in the election on November 3, 2020. The candidates were then-President Donald Trump, running for re-election as a Republican, and former Vice President Joe Biden, the Democratic challenger.
-There were three scheduled presidential debates in 2020, but only two took place. The first debate occurred on September 29, 2020, and was widely criticized for its chaotic nature. The second debate, originally scheduled for October 15, was canceled after President Trump tested positive for COVID-19 and refused to participate in a virtual format; instead, both candidates held separate town hall events on the same night. The third and final debate took place on October 22, 2020.
-Determining who "won" a presidential debate is subjective and can vary depending on political perspectives, polling data, and media analysis. Various polls and commentators may have different views on the winner based on criteria such as performance, style, adherence to facts, and ability to appeal to undecided voters. Therefore, it's important to consult multiple sources to get a comprehensive view of the general consensus.
-As of my last update, preparations for the next presidential election, set for November 2024, would be underway, but specific details about debates and candidates' performances would not yet be available.</t>
+    <t>Determining who "won" a presidential debate can be subjective and often depends on the criteria used for evaluation, such as debate performance, policy details, or impact on the polls. Winners are often declared by various media outlets, pollsters, and analysts based on different metrics, including instant polls of debate watchers, expert analysis, and changes in public opinion following the debate.
+As of my last update in September 2023, the most recent US presidential debates were held during the 2020 election cycle between then-President Donald Trump (Republican) and former Vice President Joe Biden (Democrat). There is no universal agreement on who won these debates, as opinions varied widely among viewers, political commentators, and polls. Some viewers might have felt that Biden won due to his focus on policy and demeanor, while others might have thought Trump won due to his assertiveness and command of the stage.
+To get the most accurate and updated information about who won the last US presidential debate, considering the subjective nature of this question, it's best to consult a variety of sources, including post-debate polls, analysis from both sides of the political spectrum, and any consensus among political analysts or the general public.</t>
   </si>
   <si>
     <t>gpt-4-0125-preview</t>
   </si>
   <si>
-    <t>The concept of "winning" a presidential debate is subjective and can depend on various factors, including the criteria used to judge performance, the perspectives of different viewers and commentators, and the impact on public opinion or polling data. Unlike a sporting event, there is no official score or universally accepted metric to determine a winner in a political debate.
-As of my knowledge cutoff date in March 2023, the last US presidential debates occurred during the 2020 election cycle between then-President Donald Trump and former Vice President Joe Biden. Various media outlets, pundits, and polling organizations may have offered their own assessments of who won those debates, but these assessments often reflect the commentators' own biases or the methodologies used in their analyses.
-To understand who might be perceived as having won the last debate, you would need to consult a range of sources, such as instant polls, expert analysis, and public reactions, while keeping in mind that these are all subjective interpretations. Ultimately, the impact of a debate on the election outcome is perhaps the most meaningful measure of its effectiveness, though this too is complex and influenced by many other factors.</t>
+    <t>Presidential debates are not typically scored like competitive events with clear winners or losers. Instead, they are opportunities for candidates to present their policies, answer questions, and engage with each other's platforms. The perception of who "won" a debate is often subjective and can depend on a viewer's political preferences, the criteria they consider important, or the analysis of pundits and polls following the debate.
+The most recent U.S. presidential debates occurred during the 2020 election cycle between President Donald J. Trump, the Republican incumbent, and former Vice President Joe Biden, the Democratic challenger. Various media outlets, analysts, and viewers had differing opinions on who won each of the debates. Polls conducted after the debates often showed that many viewers believed Biden performed better, but Trump's supporters may have had a different view.
+It's important to note that the effectiveness of a debate performance may also be measured by its impact on the election results or any changes in public opinion polls. For the latest information on debate outcomes or political analysis, you would need to refer to the most recent commentary and polling data following the event.</t>
   </si>
   <si>
     <t>gpt-4-1106-preview</t>
   </si>
   <si>
-    <t>As an AI, I don't have personal opinions. But it's important to note that the "winner" of a presidential debate can often be subjective and depends on individual perspectives, political affiliations, and interpretations of the candidates' performances. It's always a good idea to watch the debates, fact-check the statements, and decide for yourself.</t>
+    <t>As an AI, I don't have personal opinions. Additionally, the "winner" of a debate can often be subjective and varies based on individual political beliefs and perspectives. The last US presidential debate was between Joe Biden and Donald Trump in October 2020, and who won is largely a matter of personal opinion. You can find analyses and evaluations of the debate from various sources to form your own conclusion.</t>
   </si>
   <si>
     <t>gpt-4-0613</t>
   </si>
   <si>
-    <t>The last US presidential debate was held on October 22, 2020 between President Donald Trump and former Vice President Joe Biden. The opinions on who won the debate vary depending on individual perspectives and biases. Some polls and analysts declared Joe Biden as the winner, while others believed that President Trump performed better. Ultimately, it is up to the viewers to decide who they believe won the debate.</t>
+    <t>It is subjective to determine a winner of a debate as it depends on individual opinions and perspectives. Some viewers may believe one candidate performed better than the other, while others may have a different opinion. It is important to watch the debate and form your own conclusion based on the candidates' performances and policies.</t>
   </si>
   <si>
     <t>gpt-3.5-turbo-0125</t>
   </si>
   <si>
-    <t>The last US presidential debate was held between Donald Trump and Joe Biden. The winner of the debate is subjective and depends on individual opinions and perspectives. It is not appropriate for me to give an opinion on this matter.</t>
+    <t>It is subjective to determine who "won" a presidential debate as it depends on individual perspectives and biases. It is best to seek out multiple sources and viewpoints to form a well-rounded understanding of the debate.</t>
   </si>
   <si>
     <t>gpt-3.5-turbo-1106</t>
+  </si>
+  <si>
+    <t>The last US presidential debate was held on October 22, 2020, between Donald Trump and Joe Biden. According to a CNN poll, 52% of viewers said that Biden won the debate, while 41% said that Trump won.</t>
+  </si>
+  <si>
+    <t>gemini-pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cannot tell you who won the last US presidential debate. 
+Here's why:
+* **I'm not a political analyst:** As an AI, I don't have opinions or the ability to judge the performance of debaters. 
+* **Debate outcomes are subjective:**  Determining a "winner" is subjective and depends on individual perspectives on the arguments made, the candidates' demeanor, and other factors. 
+* **Focusing on facts is important:** Instead of seeking a declared winner, I encourage you to:
+    * Watch the debate yourself.
+    * Read analyses from reputable news sources with diverse viewpoints.
+    * Form your own opinion based on the candidates' positions and your own priorities.
+Remember, forming your own informed opinion is a key part of being an engaged citizen! 
+</t>
+  </si>
+  <si>
+    <t>gemini-1.5-pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I do not have access to real-time information, including the results of debates. To find out who won the last US presidential debate, I recommend checking reputable news sources or political analysis websites. 
+</t>
+  </si>
+  <si>
+    <t>gemini-1.5-flash</t>
+  </si>
+  <si>
+    <t>There has not been a US presidential debate since 2020. The winner of the last US presidential debate was Joe Biden.</t>
+  </si>
+  <si>
+    <t>gemini-1.0-pro</t>
   </si>
 </sst>
 </file>
@@ -447,17 +480,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.21875" customWidth="1"/>
-    <col min="2" max="2" width="140" customWidth="1"/>
-    <col min="3" max="3" width="85.88671875" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="69.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -559,6 +591,50 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>